<commit_message>
6 Easy Array Questions
</commit_message>
<xml_diff>
--- a/SDE Sheet/Leetcode DSA sheet by Fraz .xlsx
+++ b/SDE Sheet/Leetcode DSA sheet by Fraz .xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B. TECH\Coding\Practice\DSA Sheet\Fraz SDE Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B. TECH\Coding\Practice\DSA Sheet\SDE Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="354">
   <si>
     <t>Arrays</t>
   </si>
@@ -1105,17 +1105,23 @@
     <t>No.</t>
   </si>
   <si>
-    <t>DSA Sheet by FRAZ</t>
-  </si>
-  <si>
     <t>Done?</t>
+  </si>
+  <si>
+    <t>✔️</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>DSA Sheet by Rohan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1208,6 +1214,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI Emoji"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1245,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1274,6 +1292,10 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1496,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:C445"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B439" sqref="B439"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1508,7 +1530,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1516,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1531,8 +1553,11 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="17" t="s">
         <v>2</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1542,6 +1567,9 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="21" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1550,6 +1578,9 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C7" s="22" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1558,282 +1589,306 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="22" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C15" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>14</v>
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>17</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>28</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>32</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -4260,7 +4315,7 @@
     <hyperlink ref="B13" r:id="rId10"/>
     <hyperlink ref="B14" r:id="rId11"/>
     <hyperlink ref="B15" r:id="rId12"/>
-    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B19" r:id="rId13"/>
     <hyperlink ref="B20" r:id="rId14"/>
     <hyperlink ref="B21" r:id="rId15"/>
     <hyperlink ref="B22" r:id="rId16"/>
@@ -4286,292 +4341,291 @@
     <hyperlink ref="B42" r:id="rId36"/>
     <hyperlink ref="B43" r:id="rId37"/>
     <hyperlink ref="B44" r:id="rId38"/>
-    <hyperlink ref="B45" r:id="rId39"/>
-    <hyperlink ref="B48" r:id="rId40"/>
-    <hyperlink ref="B49" r:id="rId41"/>
-    <hyperlink ref="B50" r:id="rId42"/>
-    <hyperlink ref="B51" r:id="rId43"/>
-    <hyperlink ref="B52" r:id="rId44"/>
-    <hyperlink ref="B57" r:id="rId45"/>
-    <hyperlink ref="B58" r:id="rId46"/>
-    <hyperlink ref="B59" r:id="rId47"/>
-    <hyperlink ref="B60" r:id="rId48"/>
-    <hyperlink ref="B63" r:id="rId49"/>
-    <hyperlink ref="B64" r:id="rId50"/>
-    <hyperlink ref="B65" r:id="rId51"/>
-    <hyperlink ref="B66" r:id="rId52"/>
-    <hyperlink ref="B67" r:id="rId53"/>
-    <hyperlink ref="B68" r:id="rId54"/>
-    <hyperlink ref="B69" r:id="rId55"/>
-    <hyperlink ref="B70" r:id="rId56"/>
-    <hyperlink ref="B71" r:id="rId57"/>
-    <hyperlink ref="B72" r:id="rId58"/>
-    <hyperlink ref="B73" r:id="rId59"/>
-    <hyperlink ref="B74" r:id="rId60"/>
-    <hyperlink ref="B75" r:id="rId61"/>
-    <hyperlink ref="B76" r:id="rId62"/>
-    <hyperlink ref="B77" r:id="rId63"/>
-    <hyperlink ref="B78" r:id="rId64"/>
-    <hyperlink ref="B81" r:id="rId65"/>
-    <hyperlink ref="B82" r:id="rId66"/>
-    <hyperlink ref="B83" r:id="rId67"/>
-    <hyperlink ref="B84" r:id="rId68"/>
-    <hyperlink ref="B85" r:id="rId69"/>
-    <hyperlink ref="B86" r:id="rId70"/>
-    <hyperlink ref="B87" r:id="rId71"/>
-    <hyperlink ref="B88" r:id="rId72"/>
-    <hyperlink ref="B89" r:id="rId73"/>
-    <hyperlink ref="B90" r:id="rId74"/>
-    <hyperlink ref="B91" r:id="rId75"/>
-    <hyperlink ref="B92" r:id="rId76"/>
-    <hyperlink ref="B93" r:id="rId77"/>
-    <hyperlink ref="B94" r:id="rId78"/>
-    <hyperlink ref="B95" r:id="rId79"/>
-    <hyperlink ref="B100" r:id="rId80"/>
-    <hyperlink ref="B101" r:id="rId81"/>
-    <hyperlink ref="B102" r:id="rId82"/>
-    <hyperlink ref="B103" r:id="rId83"/>
-    <hyperlink ref="B104" r:id="rId84"/>
-    <hyperlink ref="B107" r:id="rId85"/>
-    <hyperlink ref="B108" r:id="rId86"/>
-    <hyperlink ref="B109" r:id="rId87"/>
-    <hyperlink ref="B110" r:id="rId88"/>
-    <hyperlink ref="B111" r:id="rId89"/>
-    <hyperlink ref="B112" r:id="rId90"/>
-    <hyperlink ref="B113" r:id="rId91"/>
-    <hyperlink ref="B114" r:id="rId92"/>
-    <hyperlink ref="B115" r:id="rId93"/>
-    <hyperlink ref="B116" r:id="rId94"/>
-    <hyperlink ref="B119" r:id="rId95"/>
-    <hyperlink ref="B120" r:id="rId96"/>
-    <hyperlink ref="B121" r:id="rId97"/>
-    <hyperlink ref="B122" r:id="rId98"/>
-    <hyperlink ref="B123" r:id="rId99"/>
-    <hyperlink ref="B124" r:id="rId100"/>
-    <hyperlink ref="B125" r:id="rId101"/>
-    <hyperlink ref="B130" r:id="rId102"/>
-    <hyperlink ref="B131" r:id="rId103"/>
-    <hyperlink ref="B132" r:id="rId104"/>
-    <hyperlink ref="B133" r:id="rId105"/>
-    <hyperlink ref="B134" r:id="rId106"/>
-    <hyperlink ref="B135" r:id="rId107"/>
-    <hyperlink ref="B136" r:id="rId108"/>
-    <hyperlink ref="B137" r:id="rId109"/>
-    <hyperlink ref="B138" r:id="rId110"/>
-    <hyperlink ref="B141" r:id="rId111"/>
-    <hyperlink ref="B142" r:id="rId112"/>
-    <hyperlink ref="B143" r:id="rId113"/>
-    <hyperlink ref="B144" r:id="rId114"/>
-    <hyperlink ref="B145" r:id="rId115"/>
-    <hyperlink ref="B146" r:id="rId116"/>
-    <hyperlink ref="B147" r:id="rId117"/>
-    <hyperlink ref="B150" r:id="rId118"/>
-    <hyperlink ref="B151" r:id="rId119"/>
-    <hyperlink ref="B152" r:id="rId120"/>
-    <hyperlink ref="B153" r:id="rId121"/>
-    <hyperlink ref="B161" r:id="rId122"/>
-    <hyperlink ref="B162" r:id="rId123"/>
-    <hyperlink ref="B163" r:id="rId124"/>
-    <hyperlink ref="B164" r:id="rId125"/>
-    <hyperlink ref="B165" r:id="rId126"/>
-    <hyperlink ref="B166" r:id="rId127"/>
-    <hyperlink ref="B167" r:id="rId128"/>
-    <hyperlink ref="B168" r:id="rId129"/>
-    <hyperlink ref="B171" r:id="rId130"/>
-    <hyperlink ref="B172" r:id="rId131"/>
-    <hyperlink ref="B173" r:id="rId132"/>
-    <hyperlink ref="B178" r:id="rId133"/>
-    <hyperlink ref="B179" r:id="rId134"/>
-    <hyperlink ref="B180" r:id="rId135"/>
-    <hyperlink ref="B181" r:id="rId136"/>
-    <hyperlink ref="B182" r:id="rId137"/>
-    <hyperlink ref="B183" r:id="rId138"/>
-    <hyperlink ref="B184" r:id="rId139"/>
-    <hyperlink ref="B185" r:id="rId140"/>
-    <hyperlink ref="B186" r:id="rId141"/>
-    <hyperlink ref="B189" r:id="rId142"/>
-    <hyperlink ref="B190" r:id="rId143"/>
-    <hyperlink ref="B191" r:id="rId144"/>
-    <hyperlink ref="B192" r:id="rId145"/>
-    <hyperlink ref="B193" r:id="rId146"/>
-    <hyperlink ref="B194" r:id="rId147"/>
-    <hyperlink ref="B195" r:id="rId148"/>
-    <hyperlink ref="B196" r:id="rId149"/>
-    <hyperlink ref="B201" r:id="rId150"/>
-    <hyperlink ref="B202" r:id="rId151"/>
-    <hyperlink ref="B203" r:id="rId152"/>
-    <hyperlink ref="B204" r:id="rId153"/>
-    <hyperlink ref="B205" r:id="rId154"/>
-    <hyperlink ref="B206" r:id="rId155"/>
-    <hyperlink ref="B207" r:id="rId156"/>
-    <hyperlink ref="B208" r:id="rId157"/>
-    <hyperlink ref="B209" r:id="rId158"/>
-    <hyperlink ref="B210" r:id="rId159"/>
-    <hyperlink ref="B211" r:id="rId160"/>
-    <hyperlink ref="B212" r:id="rId161"/>
-    <hyperlink ref="B213" r:id="rId162"/>
-    <hyperlink ref="B214" r:id="rId163"/>
-    <hyperlink ref="B215" r:id="rId164"/>
-    <hyperlink ref="B216" r:id="rId165"/>
-    <hyperlink ref="B219" r:id="rId166"/>
-    <hyperlink ref="B220" r:id="rId167"/>
-    <hyperlink ref="B221" r:id="rId168"/>
-    <hyperlink ref="B222" r:id="rId169"/>
-    <hyperlink ref="B223" r:id="rId170"/>
-    <hyperlink ref="B224" r:id="rId171"/>
-    <hyperlink ref="B225" r:id="rId172"/>
-    <hyperlink ref="B226" r:id="rId173"/>
-    <hyperlink ref="B227" r:id="rId174"/>
-    <hyperlink ref="B228" r:id="rId175"/>
-    <hyperlink ref="B229" r:id="rId176"/>
-    <hyperlink ref="B230" r:id="rId177"/>
-    <hyperlink ref="B231" r:id="rId178"/>
-    <hyperlink ref="B232" r:id="rId179"/>
-    <hyperlink ref="B233" r:id="rId180"/>
-    <hyperlink ref="B234" r:id="rId181"/>
-    <hyperlink ref="B235" r:id="rId182"/>
-    <hyperlink ref="B236" r:id="rId183"/>
-    <hyperlink ref="B239" r:id="rId184"/>
-    <hyperlink ref="B240" r:id="rId185"/>
-    <hyperlink ref="B241" r:id="rId186"/>
-    <hyperlink ref="B242" r:id="rId187"/>
-    <hyperlink ref="B243" r:id="rId188"/>
-    <hyperlink ref="B244" r:id="rId189"/>
-    <hyperlink ref="B245" r:id="rId190"/>
-    <hyperlink ref="B250" r:id="rId191"/>
-    <hyperlink ref="B251" r:id="rId192"/>
-    <hyperlink ref="B254" r:id="rId193"/>
-    <hyperlink ref="B255" r:id="rId194"/>
-    <hyperlink ref="B260" r:id="rId195"/>
-    <hyperlink ref="B261" r:id="rId196"/>
-    <hyperlink ref="B262" r:id="rId197"/>
-    <hyperlink ref="B263" r:id="rId198"/>
-    <hyperlink ref="B266" r:id="rId199"/>
-    <hyperlink ref="B267" r:id="rId200"/>
-    <hyperlink ref="B268" r:id="rId201"/>
-    <hyperlink ref="B269" r:id="rId202"/>
-    <hyperlink ref="B270" r:id="rId203"/>
-    <hyperlink ref="B271" r:id="rId204"/>
-    <hyperlink ref="B272" r:id="rId205"/>
-    <hyperlink ref="B273" r:id="rId206"/>
-    <hyperlink ref="B274" r:id="rId207"/>
-    <hyperlink ref="B277" r:id="rId208"/>
-    <hyperlink ref="B278" r:id="rId209"/>
-    <hyperlink ref="B279" r:id="rId210"/>
-    <hyperlink ref="B280" r:id="rId211"/>
-    <hyperlink ref="B281" r:id="rId212"/>
-    <hyperlink ref="B286" r:id="rId213"/>
-    <hyperlink ref="B287" r:id="rId214"/>
-    <hyperlink ref="B288" r:id="rId215"/>
-    <hyperlink ref="B289" r:id="rId216"/>
-    <hyperlink ref="B290" r:id="rId217"/>
-    <hyperlink ref="B293" r:id="rId218"/>
-    <hyperlink ref="B294" r:id="rId219"/>
-    <hyperlink ref="B295" r:id="rId220"/>
-    <hyperlink ref="B296" r:id="rId221"/>
-    <hyperlink ref="B301" r:id="rId222"/>
-    <hyperlink ref="B302" r:id="rId223"/>
-    <hyperlink ref="B303" r:id="rId224"/>
-    <hyperlink ref="B304" r:id="rId225"/>
-    <hyperlink ref="B305" r:id="rId226"/>
-    <hyperlink ref="B310" r:id="rId227"/>
-    <hyperlink ref="B311" r:id="rId228"/>
-    <hyperlink ref="B312" r:id="rId229"/>
-    <hyperlink ref="B313" r:id="rId230"/>
-    <hyperlink ref="B314" r:id="rId231"/>
-    <hyperlink ref="B315" r:id="rId232"/>
-    <hyperlink ref="B318" r:id="rId233"/>
-    <hyperlink ref="B319" r:id="rId234"/>
-    <hyperlink ref="B320" r:id="rId235"/>
-    <hyperlink ref="B321" r:id="rId236"/>
-    <hyperlink ref="B326" r:id="rId237"/>
-    <hyperlink ref="B327" r:id="rId238"/>
-    <hyperlink ref="B328" r:id="rId239"/>
-    <hyperlink ref="B329" r:id="rId240"/>
-    <hyperlink ref="B331" r:id="rId241"/>
-    <hyperlink ref="B334" r:id="rId242"/>
-    <hyperlink ref="B335" r:id="rId243"/>
-    <hyperlink ref="B336" r:id="rId244"/>
-    <hyperlink ref="B337" r:id="rId245"/>
-    <hyperlink ref="B338" r:id="rId246"/>
-    <hyperlink ref="B339" r:id="rId247"/>
-    <hyperlink ref="B340" r:id="rId248"/>
-    <hyperlink ref="B345" r:id="rId249"/>
-    <hyperlink ref="B346" r:id="rId250"/>
-    <hyperlink ref="B347" r:id="rId251"/>
-    <hyperlink ref="B348" r:id="rId252"/>
-    <hyperlink ref="B349" r:id="rId253"/>
-    <hyperlink ref="B350" r:id="rId254"/>
-    <hyperlink ref="B351" r:id="rId255"/>
-    <hyperlink ref="B356" r:id="rId256"/>
-    <hyperlink ref="B357" r:id="rId257"/>
-    <hyperlink ref="B360" r:id="rId258"/>
-    <hyperlink ref="B361" r:id="rId259"/>
-    <hyperlink ref="B362" r:id="rId260"/>
-    <hyperlink ref="B363" r:id="rId261"/>
-    <hyperlink ref="B364" r:id="rId262"/>
-    <hyperlink ref="B365" r:id="rId263"/>
-    <hyperlink ref="B366" r:id="rId264"/>
-    <hyperlink ref="B367" r:id="rId265"/>
-    <hyperlink ref="B368" r:id="rId266"/>
-    <hyperlink ref="B369" r:id="rId267"/>
-    <hyperlink ref="B370" r:id="rId268"/>
-    <hyperlink ref="B371" r:id="rId269"/>
-    <hyperlink ref="B372" r:id="rId270"/>
-    <hyperlink ref="B373" r:id="rId271"/>
-    <hyperlink ref="B376" r:id="rId272"/>
-    <hyperlink ref="B380" r:id="rId273"/>
-    <hyperlink ref="B381" r:id="rId274"/>
-    <hyperlink ref="B382" r:id="rId275"/>
-    <hyperlink ref="B383" r:id="rId276"/>
-    <hyperlink ref="B384" r:id="rId277"/>
-    <hyperlink ref="B385" r:id="rId278"/>
-    <hyperlink ref="B386" r:id="rId279"/>
-    <hyperlink ref="B387" r:id="rId280"/>
-    <hyperlink ref="B388" r:id="rId281"/>
-    <hyperlink ref="B389" r:id="rId282"/>
-    <hyperlink ref="B390" r:id="rId283"/>
-    <hyperlink ref="B391" r:id="rId284"/>
-    <hyperlink ref="B394" r:id="rId285"/>
-    <hyperlink ref="B395" r:id="rId286"/>
-    <hyperlink ref="B396" r:id="rId287"/>
-    <hyperlink ref="B397" r:id="rId288"/>
-    <hyperlink ref="B398" r:id="rId289"/>
-    <hyperlink ref="B399" r:id="rId290"/>
-    <hyperlink ref="B400" r:id="rId291"/>
-    <hyperlink ref="B401" r:id="rId292"/>
-    <hyperlink ref="B402" r:id="rId293"/>
-    <hyperlink ref="B403" r:id="rId294"/>
-    <hyperlink ref="B404" r:id="rId295"/>
-    <hyperlink ref="B405" r:id="rId296"/>
-    <hyperlink ref="B406" r:id="rId297"/>
-    <hyperlink ref="B409" r:id="rId298"/>
-    <hyperlink ref="B410" r:id="rId299"/>
-    <hyperlink ref="B414" r:id="rId300"/>
-    <hyperlink ref="B415" r:id="rId301"/>
-    <hyperlink ref="B416" r:id="rId302"/>
-    <hyperlink ref="B417" r:id="rId303"/>
-    <hyperlink ref="B418" r:id="rId304"/>
-    <hyperlink ref="B419" r:id="rId305"/>
-    <hyperlink ref="B420" r:id="rId306"/>
-    <hyperlink ref="B421" r:id="rId307"/>
-    <hyperlink ref="B424" r:id="rId308"/>
-    <hyperlink ref="B425" r:id="rId309"/>
-    <hyperlink ref="B426" r:id="rId310"/>
-    <hyperlink ref="B427" r:id="rId311"/>
-    <hyperlink ref="B428" r:id="rId312"/>
-    <hyperlink ref="B429" r:id="rId313"/>
-    <hyperlink ref="B430" r:id="rId314"/>
-    <hyperlink ref="B431" r:id="rId315"/>
-    <hyperlink ref="B432" r:id="rId316"/>
-    <hyperlink ref="B436" r:id="rId317"/>
-    <hyperlink ref="B437" r:id="rId318"/>
-    <hyperlink ref="B438" r:id="rId319"/>
-    <hyperlink ref="B439" r:id="rId320"/>
-    <hyperlink ref="B442" r:id="rId321"/>
-    <hyperlink ref="B445" r:id="rId322"/>
+    <hyperlink ref="B48" r:id="rId39"/>
+    <hyperlink ref="B49" r:id="rId40"/>
+    <hyperlink ref="B50" r:id="rId41"/>
+    <hyperlink ref="B51" r:id="rId42"/>
+    <hyperlink ref="B52" r:id="rId43"/>
+    <hyperlink ref="B57" r:id="rId44"/>
+    <hyperlink ref="B58" r:id="rId45"/>
+    <hyperlink ref="B59" r:id="rId46"/>
+    <hyperlink ref="B60" r:id="rId47"/>
+    <hyperlink ref="B63" r:id="rId48"/>
+    <hyperlink ref="B64" r:id="rId49"/>
+    <hyperlink ref="B65" r:id="rId50"/>
+    <hyperlink ref="B66" r:id="rId51"/>
+    <hyperlink ref="B67" r:id="rId52"/>
+    <hyperlink ref="B68" r:id="rId53"/>
+    <hyperlink ref="B69" r:id="rId54"/>
+    <hyperlink ref="B70" r:id="rId55"/>
+    <hyperlink ref="B71" r:id="rId56"/>
+    <hyperlink ref="B72" r:id="rId57"/>
+    <hyperlink ref="B73" r:id="rId58"/>
+    <hyperlink ref="B74" r:id="rId59"/>
+    <hyperlink ref="B75" r:id="rId60"/>
+    <hyperlink ref="B76" r:id="rId61"/>
+    <hyperlink ref="B77" r:id="rId62"/>
+    <hyperlink ref="B78" r:id="rId63"/>
+    <hyperlink ref="B81" r:id="rId64"/>
+    <hyperlink ref="B82" r:id="rId65"/>
+    <hyperlink ref="B83" r:id="rId66"/>
+    <hyperlink ref="B84" r:id="rId67"/>
+    <hyperlink ref="B85" r:id="rId68"/>
+    <hyperlink ref="B86" r:id="rId69"/>
+    <hyperlink ref="B87" r:id="rId70"/>
+    <hyperlink ref="B88" r:id="rId71"/>
+    <hyperlink ref="B89" r:id="rId72"/>
+    <hyperlink ref="B90" r:id="rId73"/>
+    <hyperlink ref="B91" r:id="rId74"/>
+    <hyperlink ref="B92" r:id="rId75"/>
+    <hyperlink ref="B93" r:id="rId76"/>
+    <hyperlink ref="B94" r:id="rId77"/>
+    <hyperlink ref="B95" r:id="rId78"/>
+    <hyperlink ref="B100" r:id="rId79"/>
+    <hyperlink ref="B101" r:id="rId80"/>
+    <hyperlink ref="B102" r:id="rId81"/>
+    <hyperlink ref="B103" r:id="rId82"/>
+    <hyperlink ref="B104" r:id="rId83"/>
+    <hyperlink ref="B107" r:id="rId84"/>
+    <hyperlink ref="B108" r:id="rId85"/>
+    <hyperlink ref="B109" r:id="rId86"/>
+    <hyperlink ref="B110" r:id="rId87"/>
+    <hyperlink ref="B111" r:id="rId88"/>
+    <hyperlink ref="B112" r:id="rId89"/>
+    <hyperlink ref="B113" r:id="rId90"/>
+    <hyperlink ref="B114" r:id="rId91"/>
+    <hyperlink ref="B115" r:id="rId92"/>
+    <hyperlink ref="B116" r:id="rId93"/>
+    <hyperlink ref="B119" r:id="rId94"/>
+    <hyperlink ref="B120" r:id="rId95"/>
+    <hyperlink ref="B121" r:id="rId96"/>
+    <hyperlink ref="B122" r:id="rId97"/>
+    <hyperlink ref="B123" r:id="rId98"/>
+    <hyperlink ref="B124" r:id="rId99"/>
+    <hyperlink ref="B125" r:id="rId100"/>
+    <hyperlink ref="B130" r:id="rId101"/>
+    <hyperlink ref="B131" r:id="rId102"/>
+    <hyperlink ref="B132" r:id="rId103"/>
+    <hyperlink ref="B133" r:id="rId104"/>
+    <hyperlink ref="B134" r:id="rId105"/>
+    <hyperlink ref="B135" r:id="rId106"/>
+    <hyperlink ref="B136" r:id="rId107"/>
+    <hyperlink ref="B137" r:id="rId108"/>
+    <hyperlink ref="B138" r:id="rId109"/>
+    <hyperlink ref="B141" r:id="rId110"/>
+    <hyperlink ref="B142" r:id="rId111"/>
+    <hyperlink ref="B143" r:id="rId112"/>
+    <hyperlink ref="B144" r:id="rId113"/>
+    <hyperlink ref="B145" r:id="rId114"/>
+    <hyperlink ref="B146" r:id="rId115"/>
+    <hyperlink ref="B147" r:id="rId116"/>
+    <hyperlink ref="B150" r:id="rId117"/>
+    <hyperlink ref="B151" r:id="rId118"/>
+    <hyperlink ref="B152" r:id="rId119"/>
+    <hyperlink ref="B153" r:id="rId120"/>
+    <hyperlink ref="B161" r:id="rId121"/>
+    <hyperlink ref="B162" r:id="rId122"/>
+    <hyperlink ref="B163" r:id="rId123"/>
+    <hyperlink ref="B164" r:id="rId124"/>
+    <hyperlink ref="B165" r:id="rId125"/>
+    <hyperlink ref="B166" r:id="rId126"/>
+    <hyperlink ref="B167" r:id="rId127"/>
+    <hyperlink ref="B168" r:id="rId128"/>
+    <hyperlink ref="B171" r:id="rId129"/>
+    <hyperlink ref="B172" r:id="rId130"/>
+    <hyperlink ref="B173" r:id="rId131"/>
+    <hyperlink ref="B178" r:id="rId132"/>
+    <hyperlink ref="B179" r:id="rId133"/>
+    <hyperlink ref="B180" r:id="rId134"/>
+    <hyperlink ref="B181" r:id="rId135"/>
+    <hyperlink ref="B182" r:id="rId136"/>
+    <hyperlink ref="B183" r:id="rId137"/>
+    <hyperlink ref="B184" r:id="rId138"/>
+    <hyperlink ref="B185" r:id="rId139"/>
+    <hyperlink ref="B186" r:id="rId140"/>
+    <hyperlink ref="B189" r:id="rId141"/>
+    <hyperlink ref="B190" r:id="rId142"/>
+    <hyperlink ref="B191" r:id="rId143"/>
+    <hyperlink ref="B192" r:id="rId144"/>
+    <hyperlink ref="B193" r:id="rId145"/>
+    <hyperlink ref="B194" r:id="rId146"/>
+    <hyperlink ref="B195" r:id="rId147"/>
+    <hyperlink ref="B196" r:id="rId148"/>
+    <hyperlink ref="B201" r:id="rId149"/>
+    <hyperlink ref="B202" r:id="rId150"/>
+    <hyperlink ref="B203" r:id="rId151"/>
+    <hyperlink ref="B204" r:id="rId152"/>
+    <hyperlink ref="B205" r:id="rId153"/>
+    <hyperlink ref="B206" r:id="rId154"/>
+    <hyperlink ref="B207" r:id="rId155"/>
+    <hyperlink ref="B208" r:id="rId156"/>
+    <hyperlink ref="B209" r:id="rId157"/>
+    <hyperlink ref="B210" r:id="rId158"/>
+    <hyperlink ref="B211" r:id="rId159"/>
+    <hyperlink ref="B212" r:id="rId160"/>
+    <hyperlink ref="B213" r:id="rId161"/>
+    <hyperlink ref="B214" r:id="rId162"/>
+    <hyperlink ref="B215" r:id="rId163"/>
+    <hyperlink ref="B216" r:id="rId164"/>
+    <hyperlink ref="B219" r:id="rId165"/>
+    <hyperlink ref="B220" r:id="rId166"/>
+    <hyperlink ref="B221" r:id="rId167"/>
+    <hyperlink ref="B222" r:id="rId168"/>
+    <hyperlink ref="B223" r:id="rId169"/>
+    <hyperlink ref="B224" r:id="rId170"/>
+    <hyperlink ref="B225" r:id="rId171"/>
+    <hyperlink ref="B226" r:id="rId172"/>
+    <hyperlink ref="B227" r:id="rId173"/>
+    <hyperlink ref="B228" r:id="rId174"/>
+    <hyperlink ref="B229" r:id="rId175"/>
+    <hyperlink ref="B230" r:id="rId176"/>
+    <hyperlink ref="B231" r:id="rId177"/>
+    <hyperlink ref="B232" r:id="rId178"/>
+    <hyperlink ref="B233" r:id="rId179"/>
+    <hyperlink ref="B234" r:id="rId180"/>
+    <hyperlink ref="B235" r:id="rId181"/>
+    <hyperlink ref="B236" r:id="rId182"/>
+    <hyperlink ref="B239" r:id="rId183"/>
+    <hyperlink ref="B240" r:id="rId184"/>
+    <hyperlink ref="B241" r:id="rId185"/>
+    <hyperlink ref="B242" r:id="rId186"/>
+    <hyperlink ref="B243" r:id="rId187"/>
+    <hyperlink ref="B244" r:id="rId188"/>
+    <hyperlink ref="B245" r:id="rId189"/>
+    <hyperlink ref="B250" r:id="rId190"/>
+    <hyperlink ref="B251" r:id="rId191"/>
+    <hyperlink ref="B254" r:id="rId192"/>
+    <hyperlink ref="B255" r:id="rId193"/>
+    <hyperlink ref="B260" r:id="rId194"/>
+    <hyperlink ref="B261" r:id="rId195"/>
+    <hyperlink ref="B262" r:id="rId196"/>
+    <hyperlink ref="B263" r:id="rId197"/>
+    <hyperlink ref="B266" r:id="rId198"/>
+    <hyperlink ref="B267" r:id="rId199"/>
+    <hyperlink ref="B268" r:id="rId200"/>
+    <hyperlink ref="B269" r:id="rId201"/>
+    <hyperlink ref="B270" r:id="rId202"/>
+    <hyperlink ref="B271" r:id="rId203"/>
+    <hyperlink ref="B272" r:id="rId204"/>
+    <hyperlink ref="B273" r:id="rId205"/>
+    <hyperlink ref="B274" r:id="rId206"/>
+    <hyperlink ref="B277" r:id="rId207"/>
+    <hyperlink ref="B278" r:id="rId208"/>
+    <hyperlink ref="B279" r:id="rId209"/>
+    <hyperlink ref="B280" r:id="rId210"/>
+    <hyperlink ref="B281" r:id="rId211"/>
+    <hyperlink ref="B286" r:id="rId212"/>
+    <hyperlink ref="B287" r:id="rId213"/>
+    <hyperlink ref="B288" r:id="rId214"/>
+    <hyperlink ref="B289" r:id="rId215"/>
+    <hyperlink ref="B290" r:id="rId216"/>
+    <hyperlink ref="B293" r:id="rId217"/>
+    <hyperlink ref="B294" r:id="rId218"/>
+    <hyperlink ref="B295" r:id="rId219"/>
+    <hyperlink ref="B296" r:id="rId220"/>
+    <hyperlink ref="B301" r:id="rId221"/>
+    <hyperlink ref="B302" r:id="rId222"/>
+    <hyperlink ref="B303" r:id="rId223"/>
+    <hyperlink ref="B304" r:id="rId224"/>
+    <hyperlink ref="B305" r:id="rId225"/>
+    <hyperlink ref="B310" r:id="rId226"/>
+    <hyperlink ref="B311" r:id="rId227"/>
+    <hyperlink ref="B312" r:id="rId228"/>
+    <hyperlink ref="B313" r:id="rId229"/>
+    <hyperlink ref="B314" r:id="rId230"/>
+    <hyperlink ref="B315" r:id="rId231"/>
+    <hyperlink ref="B318" r:id="rId232"/>
+    <hyperlink ref="B319" r:id="rId233"/>
+    <hyperlink ref="B320" r:id="rId234"/>
+    <hyperlink ref="B321" r:id="rId235"/>
+    <hyperlink ref="B326" r:id="rId236"/>
+    <hyperlink ref="B327" r:id="rId237"/>
+    <hyperlink ref="B328" r:id="rId238"/>
+    <hyperlink ref="B329" r:id="rId239"/>
+    <hyperlink ref="B331" r:id="rId240"/>
+    <hyperlink ref="B334" r:id="rId241"/>
+    <hyperlink ref="B335" r:id="rId242"/>
+    <hyperlink ref="B336" r:id="rId243"/>
+    <hyperlink ref="B337" r:id="rId244"/>
+    <hyperlink ref="B338" r:id="rId245"/>
+    <hyperlink ref="B339" r:id="rId246"/>
+    <hyperlink ref="B340" r:id="rId247"/>
+    <hyperlink ref="B345" r:id="rId248"/>
+    <hyperlink ref="B346" r:id="rId249"/>
+    <hyperlink ref="B347" r:id="rId250"/>
+    <hyperlink ref="B348" r:id="rId251"/>
+    <hyperlink ref="B349" r:id="rId252"/>
+    <hyperlink ref="B350" r:id="rId253"/>
+    <hyperlink ref="B351" r:id="rId254"/>
+    <hyperlink ref="B356" r:id="rId255"/>
+    <hyperlink ref="B357" r:id="rId256"/>
+    <hyperlink ref="B360" r:id="rId257"/>
+    <hyperlink ref="B361" r:id="rId258"/>
+    <hyperlink ref="B362" r:id="rId259"/>
+    <hyperlink ref="B363" r:id="rId260"/>
+    <hyperlink ref="B364" r:id="rId261"/>
+    <hyperlink ref="B365" r:id="rId262"/>
+    <hyperlink ref="B366" r:id="rId263"/>
+    <hyperlink ref="B367" r:id="rId264"/>
+    <hyperlink ref="B368" r:id="rId265"/>
+    <hyperlink ref="B369" r:id="rId266"/>
+    <hyperlink ref="B370" r:id="rId267"/>
+    <hyperlink ref="B371" r:id="rId268"/>
+    <hyperlink ref="B372" r:id="rId269"/>
+    <hyperlink ref="B373" r:id="rId270"/>
+    <hyperlink ref="B376" r:id="rId271"/>
+    <hyperlink ref="B380" r:id="rId272"/>
+    <hyperlink ref="B381" r:id="rId273"/>
+    <hyperlink ref="B382" r:id="rId274"/>
+    <hyperlink ref="B383" r:id="rId275"/>
+    <hyperlink ref="B384" r:id="rId276"/>
+    <hyperlink ref="B385" r:id="rId277"/>
+    <hyperlink ref="B386" r:id="rId278"/>
+    <hyperlink ref="B387" r:id="rId279"/>
+    <hyperlink ref="B388" r:id="rId280"/>
+    <hyperlink ref="B389" r:id="rId281"/>
+    <hyperlink ref="B390" r:id="rId282"/>
+    <hyperlink ref="B391" r:id="rId283"/>
+    <hyperlink ref="B394" r:id="rId284"/>
+    <hyperlink ref="B395" r:id="rId285"/>
+    <hyperlink ref="B396" r:id="rId286"/>
+    <hyperlink ref="B397" r:id="rId287"/>
+    <hyperlink ref="B398" r:id="rId288"/>
+    <hyperlink ref="B399" r:id="rId289"/>
+    <hyperlink ref="B400" r:id="rId290"/>
+    <hyperlink ref="B401" r:id="rId291"/>
+    <hyperlink ref="B402" r:id="rId292"/>
+    <hyperlink ref="B403" r:id="rId293"/>
+    <hyperlink ref="B404" r:id="rId294"/>
+    <hyperlink ref="B405" r:id="rId295"/>
+    <hyperlink ref="B406" r:id="rId296"/>
+    <hyperlink ref="B409" r:id="rId297"/>
+    <hyperlink ref="B410" r:id="rId298"/>
+    <hyperlink ref="B414" r:id="rId299"/>
+    <hyperlink ref="B415" r:id="rId300"/>
+    <hyperlink ref="B416" r:id="rId301"/>
+    <hyperlink ref="B417" r:id="rId302"/>
+    <hyperlink ref="B418" r:id="rId303"/>
+    <hyperlink ref="B419" r:id="rId304"/>
+    <hyperlink ref="B420" r:id="rId305"/>
+    <hyperlink ref="B421" r:id="rId306"/>
+    <hyperlink ref="B424" r:id="rId307"/>
+    <hyperlink ref="B425" r:id="rId308"/>
+    <hyperlink ref="B426" r:id="rId309"/>
+    <hyperlink ref="B427" r:id="rId310"/>
+    <hyperlink ref="B428" r:id="rId311"/>
+    <hyperlink ref="B429" r:id="rId312"/>
+    <hyperlink ref="B430" r:id="rId313"/>
+    <hyperlink ref="B431" r:id="rId314"/>
+    <hyperlink ref="B432" r:id="rId315"/>
+    <hyperlink ref="B436" r:id="rId316"/>
+    <hyperlink ref="B437" r:id="rId317"/>
+    <hyperlink ref="B438" r:id="rId318"/>
+    <hyperlink ref="B439" r:id="rId319"/>
+    <hyperlink ref="B442" r:id="rId320"/>
+    <hyperlink ref="B445" r:id="rId321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId323"/>
+  <pageSetup orientation="portrait" r:id="rId322"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6E Array, Arrays Easy Done
</commit_message>
<xml_diff>
--- a/SDE Sheet/Leetcode DSA sheet by Fraz .xlsx
+++ b/SDE Sheet/Leetcode DSA sheet by Fraz .xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="354">
   <si>
     <t>Arrays</t>
   </si>
@@ -1518,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:C445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1578,8 +1578,8 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>352</v>
+      <c r="C7" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,8 +1589,8 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>352</v>
+      <c r="C8" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1644,8 +1644,8 @@
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>352</v>
+      <c r="C13" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,8 +1655,8 @@
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>352</v>
+      <c r="C14" s="21" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1666,240 +1666,321 @@
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>37</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>39</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>